<commit_message>
First update to excel files
</commit_message>
<xml_diff>
--- a/backend/database/ERD.xlsx
+++ b/backend/database/ERD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="143">
   <si>
     <t>latitude</t>
   </si>
@@ -307,18 +307,12 @@
     <t>price</t>
   </si>
   <si>
-    <t>facilities</t>
-  </si>
-  <si>
     <t>equipments</t>
   </si>
   <si>
     <t>facility</t>
   </si>
   <si>
-    <t>facility_id</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -343,12 +337,6 @@
     <t>orders_equipments</t>
   </si>
   <si>
-    <t>orders_facilities</t>
-  </si>
-  <si>
-    <t>facilities_departments</t>
-  </si>
-  <si>
     <t>equipments_departments</t>
   </si>
   <si>
@@ -403,12 +391,6 @@
     <t>surname</t>
   </si>
   <si>
-    <t>ceb_meters_facilities</t>
-  </si>
-  <si>
-    <t>caesb_meters_facilities</t>
-  </si>
-  <si>
     <t>date_start</t>
   </si>
   <si>
@@ -437,6 +419,30 @@
   </si>
   <si>
     <t>items</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>equipment_category_type</t>
+  </si>
+  <si>
+    <t>ceb_meters_assets</t>
+  </si>
+  <si>
+    <t>asset_id</t>
+  </si>
+  <si>
+    <t>caesb_meters_assets</t>
+  </si>
+  <si>
+    <t>orders_assets</t>
+  </si>
+  <si>
+    <t>assets_id</t>
+  </si>
+  <si>
+    <t>assets_departments</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +538,29 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="lightDown"/>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -554,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -575,7 +604,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -890,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +936,7 @@
     <col min="1" max="1" width="1.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="1.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="3.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
@@ -977,107 +1014,107 @@
   <sheetData>
     <row r="1" spans="1:91" s="12" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
+      <c r="R1" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
       <c r="AC1" s="11"/>
-      <c r="AD1" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
+      <c r="AD1" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE1" s="21"/>
+      <c r="AF1" s="21"/>
       <c r="AG1" s="11"/>
-      <c r="AH1" s="15" t="s">
+      <c r="AH1" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
+      <c r="AI1" s="21"/>
+      <c r="AJ1" s="21"/>
       <c r="AK1" s="11"/>
-      <c r="AL1" s="14" t="s">
+      <c r="AL1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AM1" s="14"/>
-      <c r="AN1" s="14"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
       <c r="AO1" s="11"/>
-      <c r="AP1" s="14" t="s">
+      <c r="AP1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AQ1" s="14"/>
-      <c r="AR1" s="14"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19"/>
       <c r="AS1" s="11"/>
-      <c r="AT1" s="16" t="s">
+      <c r="AT1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
       <c r="AW1" s="11"/>
-      <c r="AX1" s="14" t="s">
+      <c r="AX1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="19"/>
       <c r="BA1" s="11"/>
-      <c r="BB1" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
+      <c r="BB1" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
       <c r="BE1" s="11"/>
-      <c r="BF1" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG1" s="14"/>
-      <c r="BH1" s="14"/>
+      <c r="BF1" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
       <c r="BI1" s="11"/>
-      <c r="BJ1" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="BK1" s="14"/>
-      <c r="BL1" s="14"/>
+      <c r="BJ1" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK1" s="20"/>
+      <c r="BL1" s="20"/>
       <c r="BM1" s="11"/>
-      <c r="BN1" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="BO1" s="14"/>
-      <c r="BP1" s="14"/>
+      <c r="BN1" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="BO1" s="19"/>
+      <c r="BP1" s="19"/>
       <c r="BQ1" s="11"/>
       <c r="BR1" s="13"/>
       <c r="BS1" s="11"/>
@@ -1090,41 +1127,41 @@
       <c r="BZ1" s="11"/>
       <c r="CA1" s="11"/>
       <c r="CB1" s="11"/>
-      <c r="CC1" s="14" t="s">
+      <c r="CC1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="CD1" s="14"/>
-      <c r="CE1" s="14"/>
+      <c r="CD1" s="19"/>
+      <c r="CE1" s="19"/>
       <c r="CF1" s="11"/>
-      <c r="CG1" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="CH1" s="14"/>
-      <c r="CI1" s="14"/>
+      <c r="CG1" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="CH1" s="19"/>
+      <c r="CI1" s="19"/>
       <c r="CJ1" s="11"/>
-      <c r="CK1" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="CL1" s="14"/>
-      <c r="CM1" s="14"/>
+      <c r="CK1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="CL1" s="19"/>
+      <c r="CM1" s="19"/>
     </row>
     <row r="2" spans="1:91" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="9" t="s">
@@ -1244,20 +1281,20 @@
       <c r="BH2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="BJ2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="BK2" s="7" t="s">
+      <c r="BJ2" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="BL2" s="7" t="s">
+      <c r="BL2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="BN2" s="7" t="s">
         <v>75</v>
       </c>
       <c r="BO2" s="7" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="BP2" s="7" t="s">
         <v>4</v>
@@ -1282,13 +1319,13 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="J3"/>
@@ -1299,7 +1336,7 @@
         <v>71</v>
       </c>
       <c r="O3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="P3" t="s">
         <v>4</v>
@@ -1308,7 +1345,7 @@
         <v>75</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="T3" s="7" t="s">
         <v>4</v>
@@ -1320,7 +1357,7 @@
         <v>8</v>
       </c>
       <c r="AA3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AB3" t="s">
         <v>4</v>
@@ -1329,7 +1366,7 @@
         <v>75</v>
       </c>
       <c r="AE3" s="7" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="AF3" s="7" t="s">
         <v>4</v>
@@ -1362,10 +1399,10 @@
         <v>4</v>
       </c>
       <c r="AY3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AZ3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="BB3" s="7" t="s">
         <v>75</v>
@@ -1380,18 +1417,18 @@
         <v>75</v>
       </c>
       <c r="BG3" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="BH3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ3" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK3" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="BH3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="BJ3" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="BK3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="BL3" s="7" t="s">
+      <c r="BL3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="BN3" s="7" t="s">
@@ -1412,16 +1449,16 @@
     </row>
     <row r="4" spans="1:91" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="F4"/>
-      <c r="G4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J4"/>
@@ -1441,7 +1478,7 @@
         <v>23</v>
       </c>
       <c r="X4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AA4" t="s">
         <v>81</v>
@@ -1456,13 +1493,13 @@
         <v>8</v>
       </c>
       <c r="AM4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AN4" t="s">
         <v>4</v>
       </c>
       <c r="AQ4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AR4" t="s">
         <v>4</v>
@@ -1475,13 +1512,13 @@
         <v>78</v>
       </c>
       <c r="AY4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="AZ4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="BC4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="BD4" t="s">
         <v>4</v>
@@ -1500,11 +1537,11 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="F5"/>
-      <c r="G5" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J5"/>
@@ -1548,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="AQ5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AR5" t="s">
         <v>4</v>
@@ -1561,10 +1598,10 @@
         <v>78</v>
       </c>
       <c r="AY5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AZ5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="BB5" s="8"/>
       <c r="BC5" s="8" t="s">
@@ -1581,19 +1618,19 @@
       </c>
     </row>
     <row r="6" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>107</v>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="J6"/>
       <c r="K6" t="s">
@@ -1630,7 +1667,7 @@
         <v>8</v>
       </c>
       <c r="AQ6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="AR6" t="s">
         <v>4</v>
@@ -1666,16 +1703,16 @@
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J7"/>
       <c r="K7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L7" t="s">
         <v>4</v>
@@ -1714,7 +1751,7 @@
         <v>4</v>
       </c>
       <c r="AY7" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="AZ7" s="3" t="s">
         <v>8</v>
@@ -1734,16 +1771,16 @@
       <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J8"/>
       <c r="K8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L8" t="s">
         <v>4</v>
@@ -1776,7 +1813,7 @@
         <v>8</v>
       </c>
       <c r="AY8" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="AZ8" s="3" t="s">
         <v>4</v>
@@ -1796,11 +1833,11 @@
       <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="17" t="s">
         <v>4</v>
       </c>
       <c r="O9" t="s">
@@ -1822,16 +1859,16 @@
         <v>8</v>
       </c>
       <c r="AQ9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AR9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="AX9" s="7" t="s">
         <v>75</v>
       </c>
       <c r="AY9" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="AZ9" s="7" t="s">
         <v>4</v>
@@ -1844,14 +1881,18 @@
       </c>
     </row>
     <row r="10" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="O10" t="s">
@@ -1879,21 +1920,25 @@
         <v>75</v>
       </c>
       <c r="AY10" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="AZ10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="O11" t="s">
@@ -1919,23 +1964,27 @@
       <c r="AR11" s="3"/>
       <c r="AX11" s="3"/>
       <c r="AY11" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AZ11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="18" t="s">
         <v>4</v>
       </c>
       <c r="O12" t="s">
@@ -1958,16 +2007,20 @@
       </c>
       <c r="AX12" s="3"/>
       <c r="AY12" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="AZ12" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="O13" t="s">
         <v>25</v>
       </c>
@@ -1988,16 +2041,20 @@
       </c>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AZ13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="W14" t="s">
         <v>35</v>
       </c>
@@ -2012,16 +2069,20 @@
       </c>
       <c r="AX14" s="3"/>
       <c r="AY14" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="AZ14" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="W15" t="s">
         <v>36</v>
       </c>
@@ -2036,7 +2097,7 @@
       </c>
       <c r="AX15" s="3"/>
       <c r="AY15" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="AZ15" s="3" t="s">
         <v>4</v>
@@ -2059,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="AY16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AZ16" t="s">
         <v>6</v>
@@ -2102,7 +2163,7 @@
         <v>6</v>
       </c>
       <c r="AY18" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="AZ18" s="3" t="s">
         <v>78</v>
@@ -2116,7 +2177,7 @@
         <v>8</v>
       </c>
       <c r="AY19" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="AZ19" s="3" t="s">
         <v>78</v>
@@ -2270,8 +2331,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="BN1:BP1"/>
     <mergeCell ref="BB1:BD1"/>
     <mergeCell ref="AT1:AV1"/>
@@ -2290,6 +2349,8 @@
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="AH1:AJ1"/>
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AX1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remake tables in Excel files
</commit_message>
<xml_diff>
--- a/backend/database/ERD.xlsx
+++ b/backend/database/ERD.xlsx
@@ -385,9 +385,6 @@
     <t>meter_name</t>
   </si>
   <si>
-    <t>modtar_type</t>
-  </si>
-  <si>
     <t>surname</t>
   </si>
   <si>
@@ -443,6 +440,9 @@
   </si>
   <si>
     <t>assets_departments</t>
+  </si>
+  <si>
+    <t>modtar_text</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +561,12 @@
         <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -583,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -612,15 +618,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AZ3" sqref="AZ3:AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,16 +1022,16 @@
     <row r="1" spans="1:91" s="12" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
       <c r="I1" s="11"/>
       <c r="J1" s="19" t="s">
         <v>21</v>
@@ -1038,17 +1045,17 @@
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
+      <c r="R1" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
       <c r="Y1" s="11"/>
       <c r="Z1" s="19" t="s">
         <v>11</v>
@@ -1056,17 +1063,17 @@
       <c r="AA1" s="19"/>
       <c r="AB1" s="19"/>
       <c r="AC1" s="11"/>
-      <c r="AD1" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
+      <c r="AD1" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
       <c r="AG1" s="11"/>
-      <c r="AH1" s="21" t="s">
+      <c r="AH1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
       <c r="AK1" s="11"/>
       <c r="AL1" s="19" t="s">
         <v>13</v>
@@ -1080,11 +1087,11 @@
       <c r="AQ1" s="19"/>
       <c r="AR1" s="19"/>
       <c r="AS1" s="11"/>
-      <c r="AT1" s="22" t="s">
+      <c r="AT1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
+      <c r="AU1" s="20"/>
+      <c r="AV1" s="20"/>
       <c r="AW1" s="11"/>
       <c r="AX1" s="19" t="s">
         <v>19</v>
@@ -1093,25 +1100,25 @@
       <c r="AZ1" s="19"/>
       <c r="BA1" s="11"/>
       <c r="BB1" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BC1" s="19"/>
       <c r="BD1" s="19"/>
       <c r="BE1" s="11"/>
       <c r="BF1" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BG1" s="19"/>
       <c r="BH1" s="19"/>
       <c r="BI1" s="11"/>
-      <c r="BJ1" s="20" t="s">
+      <c r="BJ1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
+      <c r="BK1" s="21"/>
+      <c r="BL1" s="21"/>
       <c r="BM1" s="11"/>
       <c r="BN1" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BO1" s="19"/>
       <c r="BP1" s="19"/>
@@ -1134,7 +1141,7 @@
       <c r="CE1" s="19"/>
       <c r="CF1" s="11"/>
       <c r="CG1" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CH1" s="19"/>
       <c r="CI1" s="19"/>
@@ -1150,7 +1157,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>4</v>
@@ -1294,7 +1301,7 @@
         <v>75</v>
       </c>
       <c r="BO2" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BP2" s="7" t="s">
         <v>4</v>
@@ -1345,7 +1352,7 @@
         <v>75</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T3" s="7" t="s">
         <v>4</v>
@@ -1366,7 +1373,7 @@
         <v>75</v>
       </c>
       <c r="AE3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AF3" s="7" t="s">
         <v>4</v>
@@ -1417,7 +1424,7 @@
         <v>75</v>
       </c>
       <c r="BG3" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BH3" s="7" t="s">
         <v>4</v>
@@ -1474,11 +1481,11 @@
       <c r="P4" t="s">
         <v>4</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="X4" t="s">
-        <v>123</v>
+      <c r="X4" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="AA4" t="s">
         <v>81</v>
@@ -1518,7 +1525,7 @@
         <v>113</v>
       </c>
       <c r="BC4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="BD4" t="s">
         <v>4</v>
@@ -1551,11 +1558,11 @@
       <c r="L5" t="s">
         <v>71</v>
       </c>
-      <c r="O5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P5" t="s">
-        <v>23</v>
+      <c r="O5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="P5" s="23" t="s">
+        <v>4</v>
       </c>
       <c r="W5" t="s">
         <v>26</v>
@@ -1585,7 +1592,7 @@
         <v>5</v>
       </c>
       <c r="AQ5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AR5" t="s">
         <v>4</v>
@@ -1667,7 +1674,7 @@
         <v>8</v>
       </c>
       <c r="AQ6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR6" t="s">
         <v>4</v>
@@ -1810,7 +1817,7 @@
         <v>85</v>
       </c>
       <c r="AR8" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AY8" s="3" t="s">
         <v>116</v>
@@ -1886,7 +1893,7 @@
         <v>101</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17" t="s">
@@ -1964,7 +1971,7 @@
       <c r="AR11" s="3"/>
       <c r="AX11" s="3"/>
       <c r="AY11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AZ11" s="3" t="s">
         <v>4</v>
@@ -2007,7 +2014,7 @@
       </c>
       <c r="AX12" s="3"/>
       <c r="AY12" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AZ12" s="3" t="s">
         <v>4</v>
@@ -2041,7 +2048,7 @@
       </c>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AZ13" s="3" t="s">
         <v>4</v>
@@ -2069,7 +2076,7 @@
       </c>
       <c r="AX14" s="3"/>
       <c r="AY14" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AZ14" s="3" t="s">
         <v>4</v>
@@ -2097,7 +2104,7 @@
       </c>
       <c r="AX15" s="3"/>
       <c r="AY15" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AZ15" s="3" t="s">
         <v>4</v>
@@ -2177,7 +2184,7 @@
         <v>8</v>
       </c>
       <c r="AY19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AZ19" s="3" t="s">
         <v>78</v>
@@ -2331,14 +2338,8 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="AT1:AV1"/>
-    <mergeCell ref="BJ1:BL1"/>
-    <mergeCell ref="CK1:CM1"/>
-    <mergeCell ref="BF1:BH1"/>
-    <mergeCell ref="CG1:CI1"/>
-    <mergeCell ref="CC1:CE1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Z1:AB1"/>
@@ -2349,8 +2350,14 @@
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="AH1:AJ1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AX1:AZ1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="AT1:AV1"/>
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="CK1:CM1"/>
+    <mergeCell ref="BF1:BH1"/>
+    <mergeCell ref="CG1:CI1"/>
+    <mergeCell ref="CC1:CE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete rebuild of database (db name: cmms2)
</commit_message>
<xml_diff>
--- a/backend/database/ERD.xlsx
+++ b/backend/database/ERD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="143">
   <si>
     <t>latitude</t>
   </si>
@@ -232,9 +232,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -443,6 +440,9 @@
   </si>
   <si>
     <t>modtar_text</t>
+  </si>
+  <si>
+    <t>password_hash</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,6 +567,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -589,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -615,6 +621,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,7 +635,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AZ3" sqref="AZ3:AZ5"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AU4" sqref="AU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,107 +1028,107 @@
   <sheetData>
     <row r="1" spans="1:91" s="12" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="F1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="11"/>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
+      <c r="R1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="22" t="s">
+      <c r="V1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
       <c r="Y1" s="11"/>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
+      <c r="AA1" s="21"/>
+      <c r="AB1" s="21"/>
       <c r="AC1" s="11"/>
-      <c r="AD1" s="22" t="s">
+      <c r="AD1" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM1" s="21"/>
+      <c r="AN1" s="21"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ1" s="21"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="BC1" s="21"/>
+      <c r="BD1" s="21"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="19"/>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="11"/>
-      <c r="AX1" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AY1" s="19"/>
-      <c r="AZ1" s="19"/>
-      <c r="BA1" s="11"/>
-      <c r="BB1" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="BC1" s="19"/>
-      <c r="BD1" s="19"/>
-      <c r="BE1" s="11"/>
-      <c r="BF1" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="BG1" s="19"/>
-      <c r="BH1" s="19"/>
+      <c r="BG1" s="21"/>
+      <c r="BH1" s="21"/>
       <c r="BI1" s="11"/>
-      <c r="BJ1" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="BK1" s="21"/>
-      <c r="BL1" s="21"/>
+      <c r="BJ1" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK1" s="23"/>
+      <c r="BL1" s="23"/>
       <c r="BM1" s="11"/>
-      <c r="BN1" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="BO1" s="19"/>
-      <c r="BP1" s="19"/>
+      <c r="BN1" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="BO1" s="21"/>
+      <c r="BP1" s="21"/>
       <c r="BQ1" s="11"/>
       <c r="BR1" s="13"/>
       <c r="BS1" s="11"/>
@@ -1134,30 +1141,30 @@
       <c r="BZ1" s="11"/>
       <c r="CA1" s="11"/>
       <c r="CB1" s="11"/>
-      <c r="CC1" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="CD1" s="19"/>
-      <c r="CE1" s="19"/>
+      <c r="CC1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="CD1" s="21"/>
+      <c r="CE1" s="21"/>
       <c r="CF1" s="11"/>
-      <c r="CG1" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="CH1" s="19"/>
-      <c r="CI1" s="19"/>
+      <c r="CG1" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="CH1" s="21"/>
+      <c r="CI1" s="21"/>
       <c r="CJ1" s="11"/>
-      <c r="CK1" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="CL1" s="19"/>
-      <c r="CM1" s="19"/>
+      <c r="CK1" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="CL1" s="21"/>
+      <c r="CM1" s="21"/>
     </row>
     <row r="2" spans="1:91" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>4</v>
@@ -1166,7 +1173,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>4</v>
@@ -1190,7 +1197,7 @@
         <v>8</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>7</v>
@@ -1199,7 +1206,7 @@
         <v>8</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>7</v>
@@ -1217,7 +1224,7 @@
         <v>8</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AE2" s="7" t="s">
         <v>7</v>
@@ -1226,7 +1233,7 @@
         <v>8</v>
       </c>
       <c r="AH2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AI2" s="7" t="s">
         <v>7</v>
@@ -1253,7 +1260,7 @@
         <v>8</v>
       </c>
       <c r="AT2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AU2" s="7" t="s">
         <v>15</v>
@@ -1271,7 +1278,7 @@
         <v>8</v>
       </c>
       <c r="BB2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BC2" s="7" t="s">
         <v>20</v>
@@ -1280,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="BF2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BG2" s="7" t="s">
         <v>20</v>
@@ -1289,7 +1296,7 @@
         <v>8</v>
       </c>
       <c r="BJ2" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BK2" s="18" t="s">
         <v>20</v>
@@ -1298,16 +1305,16 @@
         <v>8</v>
       </c>
       <c r="BN2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BO2" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BP2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="CG2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="CH2" s="7" t="s">
         <v>22</v>
@@ -1318,19 +1325,19 @@
     </row>
     <row r="3" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="15" t="s">
         <v>4</v>
@@ -1343,16 +1350,16 @@
         <v>71</v>
       </c>
       <c r="O3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P3" t="s">
         <v>4</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T3" s="7" t="s">
         <v>4</v>
@@ -1364,16 +1371,16 @@
         <v>8</v>
       </c>
       <c r="AA3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AB3" t="s">
         <v>4</v>
       </c>
       <c r="AD3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AE3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF3" s="7" t="s">
         <v>4</v>
@@ -1385,34 +1392,34 @@
         <v>8</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AN3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="AQ3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AR3" t="s">
         <v>4</v>
       </c>
       <c r="AU3" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="AV3" t="s">
         <v>4</v>
       </c>
       <c r="AY3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ3" t="s">
         <v>110</v>
       </c>
-      <c r="AZ3" t="s">
-        <v>111</v>
-      </c>
       <c r="BB3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BC3" s="7" t="s">
         <v>15</v>
@@ -1421,25 +1428,25 @@
         <v>8</v>
       </c>
       <c r="BF3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BG3" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BH3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="BJ3" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BK3" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BL3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="BN3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BO3" s="7" t="s">
         <v>14</v>
@@ -1448,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="CH3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="CI3" t="s">
         <v>4</v>
@@ -1456,14 +1463,14 @@
     </row>
     <row r="4" spans="1:91" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="16" t="s">
         <v>4</v>
@@ -1476,19 +1483,19 @@
         <v>71</v>
       </c>
       <c r="O4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P4" t="s">
         <v>4</v>
       </c>
-      <c r="W4" s="23" t="s">
+      <c r="W4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="23" t="s">
+      <c r="X4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="AA4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AB4" t="s">
         <v>4</v>
@@ -1500,38 +1507,38 @@
         <v>8</v>
       </c>
       <c r="AM4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AN4" t="s">
         <v>4</v>
       </c>
       <c r="AQ4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AR4" t="s">
         <v>4</v>
       </c>
       <c r="AT4" s="8"/>
       <c r="AU4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AV4" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AY4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ4" t="s">
         <v>112</v>
       </c>
-      <c r="AZ4" t="s">
-        <v>113</v>
-      </c>
       <c r="BC4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BD4" t="s">
         <v>4</v>
       </c>
       <c r="CH4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="CI4" t="s">
         <v>4</v>
@@ -1539,29 +1546,29 @@
     </row>
     <row r="5" spans="1:91" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J5"/>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L5" t="s">
         <v>71</v>
       </c>
-      <c r="O5" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="P5" s="23" t="s">
+      <c r="O5" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="P5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="W5" t="s">
@@ -1571,10 +1578,10 @@
         <v>71</v>
       </c>
       <c r="Z5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AB5" s="7" t="s">
         <v>4</v>
@@ -1592,65 +1599,65 @@
         <v>5</v>
       </c>
       <c r="AQ5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AR5" t="s">
         <v>4</v>
       </c>
       <c r="AT5" s="8"/>
       <c r="AU5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV5" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AV5" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="AY5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AZ5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BB5" s="8"/>
       <c r="BC5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BD5" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="CH5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="CI5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J6"/>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
         <v>4</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>4</v>
@@ -1674,29 +1681,29 @@
         <v>8</v>
       </c>
       <c r="AQ6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AR6" t="s">
         <v>4</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AZ6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="BB6" s="8"/>
       <c r="BC6" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD6" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="BD6" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="CH6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="CI6" t="s">
         <v>6</v>
@@ -1712,20 +1719,20 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J7"/>
       <c r="K7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L7" t="s">
         <v>4</v>
       </c>
       <c r="O7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P7" t="s">
         <v>4</v>
@@ -1749,22 +1756,22 @@
         <v>71</v>
       </c>
       <c r="AP7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AQ7" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AR7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="AY7" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AZ7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="CH7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="CI7" t="s">
         <v>6</v>
@@ -1780,20 +1787,20 @@
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J8"/>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L8" t="s">
         <v>4</v>
       </c>
       <c r="O8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P8" t="s">
         <v>4</v>
@@ -1811,22 +1818,22 @@
         <v>8</v>
       </c>
       <c r="AP8" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AQ8" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AR8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="AY8" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AZ8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="CH8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="CI8" t="s">
         <v>4</v>
@@ -1848,7 +1855,7 @@
         <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P9" t="s">
         <v>4</v>
@@ -1866,22 +1873,22 @@
         <v>8</v>
       </c>
       <c r="AQ9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AR9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AX9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AY9" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AZ9" s="7" t="s">
         <v>4</v>
       </c>
       <c r="CH9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="CI9" t="s">
         <v>6</v>
@@ -1890,20 +1897,20 @@
     <row r="10" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P10" t="s">
         <v>4</v>
@@ -1924,10 +1931,10 @@
       <c r="AQ10" s="3"/>
       <c r="AR10" s="3"/>
       <c r="AX10" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AY10" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AZ10" s="7" t="s">
         <v>4</v>
@@ -1936,20 +1943,20 @@
     <row r="11" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="O11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P11" t="s">
         <v>4</v>
@@ -1971,7 +1978,7 @@
       <c r="AR11" s="3"/>
       <c r="AX11" s="3"/>
       <c r="AY11" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ11" s="3" t="s">
         <v>4</v>
@@ -1980,16 +1987,16 @@
     <row r="12" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>4</v>
@@ -2014,7 +2021,7 @@
       </c>
       <c r="AX12" s="3"/>
       <c r="AY12" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AZ12" s="3" t="s">
         <v>4</v>
@@ -2048,7 +2055,7 @@
       </c>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AZ13" s="3" t="s">
         <v>4</v>
@@ -2057,7 +2064,7 @@
     <row r="14" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>6</v>
@@ -2076,7 +2083,7 @@
       </c>
       <c r="AX14" s="3"/>
       <c r="AY14" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AZ14" s="3" t="s">
         <v>4</v>
@@ -2085,7 +2092,7 @@
     <row r="15" spans="1:91" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>4</v>
@@ -2104,7 +2111,7 @@
       </c>
       <c r="AX15" s="3"/>
       <c r="AY15" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AZ15" s="3" t="s">
         <v>4</v>
@@ -2127,7 +2134,7 @@
         <v>6</v>
       </c>
       <c r="AY16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AZ16" t="s">
         <v>6</v>
@@ -2150,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="AY17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AZ17" s="3" t="s">
         <v>4</v>
@@ -2170,10 +2177,10 @@
         <v>6</v>
       </c>
       <c r="AY18" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AZ18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:52" x14ac:dyDescent="0.25">
@@ -2184,10 +2191,10 @@
         <v>8</v>
       </c>
       <c r="AY19" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AZ19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="2:52" x14ac:dyDescent="0.25">
@@ -2199,10 +2206,10 @@
       </c>
       <c r="AX20" s="8"/>
       <c r="AY20" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AZ20" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="2:52" x14ac:dyDescent="0.25">
@@ -2212,8 +2219,15 @@
       <c r="X21" t="s">
         <v>8</v>
       </c>
-      <c r="AY21" s="3"/>
-      <c r="AZ21" s="3"/>
+      <c r="AX21" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY21" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ21" s="20" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="2:52" x14ac:dyDescent="0.25">
       <c r="W22" t="s">

</xml_diff>

<commit_message>
Change column name to is_active
</commit_message>
<xml_diff>
--- a/backend/database/ERD.xlsx
+++ b/backend/database/ERD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="144">
   <si>
     <t>latitude</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>password_hash</t>
+  </si>
+  <si>
+    <t>is_active</t>
   </si>
 </sst>
 </file>
@@ -626,13 +629,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -942,7 +945,7 @@
   <dimension ref="A1:CM62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AU4" sqref="AU4"/>
+      <selection activeCell="AU7" sqref="AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,11 +1037,11 @@
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
       <c r="I1" s="11"/>
       <c r="J1" s="21" t="s">
         <v>21</v>
@@ -1052,17 +1055,17 @@
       <c r="O1" s="21"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
       <c r="Y1" s="11"/>
       <c r="Z1" s="21" t="s">
         <v>11</v>
@@ -1070,17 +1073,17 @@
       <c r="AA1" s="21"/>
       <c r="AB1" s="21"/>
       <c r="AC1" s="11"/>
-      <c r="AD1" s="24" t="s">
+      <c r="AD1" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
       <c r="AG1" s="11"/>
-      <c r="AH1" s="24" t="s">
+      <c r="AH1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
       <c r="AK1" s="11"/>
       <c r="AL1" s="21" t="s">
         <v>13</v>
@@ -1094,11 +1097,11 @@
       <c r="AQ1" s="21"/>
       <c r="AR1" s="21"/>
       <c r="AS1" s="11"/>
-      <c r="AT1" s="22" t="s">
+      <c r="AT1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
       <c r="AW1" s="11"/>
       <c r="AX1" s="21" t="s">
         <v>19</v>
@@ -1118,11 +1121,11 @@
       <c r="BG1" s="21"/>
       <c r="BH1" s="21"/>
       <c r="BI1" s="11"/>
-      <c r="BJ1" s="23" t="s">
+      <c r="BJ1" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="BK1" s="23"/>
-      <c r="BL1" s="23"/>
+      <c r="BK1" s="22"/>
+      <c r="BL1" s="22"/>
       <c r="BM1" s="11"/>
       <c r="BN1" s="21" t="s">
         <v>140</v>
@@ -1686,6 +1689,12 @@
       <c r="AR6" t="s">
         <v>4</v>
       </c>
+      <c r="AU6" t="s">
+        <v>143</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>5</v>
+      </c>
       <c r="AX6" s="1" t="s">
         <v>74</v>
       </c>
@@ -2352,6 +2361,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="AT1:AV1"/>
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="CK1:CM1"/>
+    <mergeCell ref="BF1:BH1"/>
+    <mergeCell ref="CG1:CI1"/>
+    <mergeCell ref="CC1:CE1"/>
     <mergeCell ref="AP1:AR1"/>
     <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="B1:D1"/>
@@ -2364,14 +2381,6 @@
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="AH1:AJ1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="AT1:AV1"/>
-    <mergeCell ref="BJ1:BL1"/>
-    <mergeCell ref="CK1:CM1"/>
-    <mergeCell ref="BF1:BH1"/>
-    <mergeCell ref="CG1:CI1"/>
-    <mergeCell ref="CC1:CE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change table assets (add place column)
</commit_message>
<xml_diff>
--- a/backend/database/ERD.xlsx
+++ b/backend/database/ERD.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="145">
   <si>
     <t>latitude</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>is_active</t>
+  </si>
+  <si>
+    <t>place</t>
   </si>
 </sst>
 </file>
@@ -629,13 +632,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AU7" sqref="AU7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,11 +1040,11 @@
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="11"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="11"/>
       <c r="J1" s="21" t="s">
         <v>21</v>
@@ -1055,17 +1058,17 @@
       <c r="O1" s="21"/>
       <c r="P1" s="21"/>
       <c r="Q1" s="11"/>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
       <c r="Y1" s="11"/>
       <c r="Z1" s="21" t="s">
         <v>11</v>
@@ -1073,17 +1076,17 @@
       <c r="AA1" s="21"/>
       <c r="AB1" s="21"/>
       <c r="AC1" s="11"/>
-      <c r="AD1" s="23" t="s">
+      <c r="AD1" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
       <c r="AG1" s="11"/>
-      <c r="AH1" s="23" t="s">
+      <c r="AH1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
       <c r="AK1" s="11"/>
       <c r="AL1" s="21" t="s">
         <v>13</v>
@@ -1097,11 +1100,11 @@
       <c r="AQ1" s="21"/>
       <c r="AR1" s="21"/>
       <c r="AS1" s="11"/>
-      <c r="AT1" s="24" t="s">
+      <c r="AT1" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="AU1" s="24"/>
-      <c r="AV1" s="24"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
       <c r="AW1" s="11"/>
       <c r="AX1" s="21" t="s">
         <v>19</v>
@@ -1121,11 +1124,11 @@
       <c r="BG1" s="21"/>
       <c r="BH1" s="21"/>
       <c r="BI1" s="11"/>
-      <c r="BJ1" s="22" t="s">
+      <c r="BJ1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22"/>
+      <c r="BK1" s="23"/>
+      <c r="BL1" s="23"/>
       <c r="BM1" s="11"/>
       <c r="BN1" s="21" t="s">
         <v>140</v>
@@ -2127,9 +2130,15 @@
       </c>
     </row>
     <row r="16" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="W16" t="s">
         <v>37</v>
       </c>
@@ -2361,14 +2370,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="BN1:BP1"/>
-    <mergeCell ref="BB1:BD1"/>
-    <mergeCell ref="AT1:AV1"/>
-    <mergeCell ref="BJ1:BL1"/>
-    <mergeCell ref="CK1:CM1"/>
-    <mergeCell ref="BF1:BH1"/>
-    <mergeCell ref="CG1:CI1"/>
-    <mergeCell ref="CC1:CE1"/>
     <mergeCell ref="AP1:AR1"/>
     <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="B1:D1"/>
@@ -2381,6 +2382,14 @@
     <mergeCell ref="V1:X1"/>
     <mergeCell ref="AH1:AJ1"/>
     <mergeCell ref="J1:L1"/>
+    <mergeCell ref="BN1:BP1"/>
+    <mergeCell ref="BB1:BD1"/>
+    <mergeCell ref="AT1:AV1"/>
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="CK1:CM1"/>
+    <mergeCell ref="BF1:BH1"/>
+    <mergeCell ref="CG1:CI1"/>
+    <mergeCell ref="CC1:CE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>